<commit_message>
presolve off for highs
</commit_message>
<xml_diff>
--- a/export/MGS_export.xlsx
+++ b/export/MGS_export.xlsx
@@ -537,7 +537,7 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -629,13 +629,13 @@
         <v>4</v>
       </c>
       <c r="D10">
-        <v>-0</v>
+        <v>1.304457284609194E-08</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1.304457284609194E-08</v>
       </c>
       <c r="F10" s="1">
-        <v>0</v>
+        <v>6.009114365778562E-14</v>
       </c>
       <c r="G10">
         <v>2181.697</v>
@@ -652,13 +652,13 @@
         <v>4</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>2181</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>2181.000000013044</v>
       </c>
       <c r="F11" s="1">
-        <v>0</v>
+        <v>0.01004699700517052</v>
       </c>
       <c r="G11">
         <v>2181.697</v>
@@ -675,13 +675,13 @@
         <v>4</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>2181</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>4362.000000013045</v>
       </c>
       <c r="F12" s="1">
-        <v>0</v>
+        <v>0.02009399401028094</v>
       </c>
       <c r="G12">
         <v>2181.697</v>
@@ -698,13 +698,13 @@
         <v>4</v>
       </c>
       <c r="D13">
-        <v>-0</v>
+        <v>2181</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>6543.000000013045</v>
       </c>
       <c r="F13" s="1">
-        <v>0</v>
+        <v>0.03014099101539137</v>
       </c>
       <c r="G13">
         <v>2181.697</v>
@@ -724,10 +724,10 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>6543.000000013045</v>
       </c>
       <c r="F14" s="1">
-        <v>0</v>
+        <v>0.03014099101539137</v>
       </c>
       <c r="G14">
         <v>2181.697</v>
@@ -747,10 +747,10 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>6543.000000013045</v>
       </c>
       <c r="F15" s="1">
-        <v>0</v>
+        <v>0.03014099101539137</v>
       </c>
       <c r="G15">
         <v>2181.697</v>
@@ -770,10 +770,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>6543.000000013045</v>
       </c>
       <c r="F16" s="1">
-        <v>0</v>
+        <v>0.03014099101539137</v>
       </c>
       <c r="G16">
         <v>2181.697</v>
@@ -793,10 +793,10 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>6543.000000013045</v>
       </c>
       <c r="F17" s="1">
-        <v>0</v>
+        <v>0.03014099101539137</v>
       </c>
       <c r="G17">
         <v>2181.697</v>
@@ -816,10 +816,10 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>6543.000000013045</v>
       </c>
       <c r="F18" s="1">
-        <v>0</v>
+        <v>0.03014099101539137</v>
       </c>
       <c r="G18">
         <v>2181.697</v>
@@ -839,10 +839,10 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>6543.000000013045</v>
       </c>
       <c r="F19" s="1">
-        <v>0</v>
+        <v>0.03014099101539137</v>
       </c>
       <c r="G19">
         <v>2181.697</v>
@@ -862,10 +862,10 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>6543.000000013045</v>
       </c>
       <c r="F20" s="1">
-        <v>0</v>
+        <v>0.03014099101539137</v>
       </c>
       <c r="G20">
         <v>2181.697</v>
@@ -885,10 +885,10 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>6543.000000013045</v>
       </c>
       <c r="F21" s="1">
-        <v>0</v>
+        <v>0.03014099101539137</v>
       </c>
       <c r="G21">
         <v>2181.697</v>
@@ -908,10 +908,10 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>6543.000000013045</v>
       </c>
       <c r="F22" s="1">
-        <v>0</v>
+        <v>0.03014099101539137</v>
       </c>
       <c r="G22">
         <v>2181.697</v>
@@ -928,13 +928,13 @@
         <v>4</v>
       </c>
       <c r="D23">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>6543.000000013045</v>
       </c>
       <c r="F23" s="1">
-        <v>0</v>
+        <v>0.03014099101539137</v>
       </c>
       <c r="G23">
         <v>2181.697</v>
@@ -954,10 +954,10 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>6543.000000013045</v>
       </c>
       <c r="F24" s="1">
-        <v>0</v>
+        <v>0.03014099101539137</v>
       </c>
       <c r="G24">
         <v>2181.697</v>
@@ -977,10 +977,10 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>6543.000000013045</v>
       </c>
       <c r="F25" s="1">
-        <v>0</v>
+        <v>0.03014099101539137</v>
       </c>
       <c r="G25">
         <v>2181.697</v>
@@ -1000,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>6543.000000013045</v>
       </c>
       <c r="F26" s="1">
-        <v>0</v>
+        <v>0.03014099101539137</v>
       </c>
       <c r="G26">
         <v>2181.697</v>
@@ -1023,10 +1023,10 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>6543.000000013045</v>
       </c>
       <c r="F27" s="1">
-        <v>0</v>
+        <v>0.03014099101539137</v>
       </c>
       <c r="G27">
         <v>2181.697</v>
@@ -1046,10 +1046,10 @@
         <v>2130</v>
       </c>
       <c r="E28">
-        <v>2130</v>
+        <v>8673.000000013044</v>
       </c>
       <c r="F28" s="1">
-        <v>0.009812060348869878</v>
+        <v>0.03995305136426124</v>
       </c>
       <c r="G28">
         <v>2181.697</v>
@@ -1066,13 +1066,13 @@
         <v>4</v>
       </c>
       <c r="D29">
-        <v>2181</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>4311</v>
+        <v>8673.000000013044</v>
       </c>
       <c r="F29" s="1">
-        <v>0.0198590573539803</v>
+        <v>0.03995305136426124</v>
       </c>
       <c r="G29">
         <v>2181.697</v>
@@ -1089,13 +1089,13 @@
         <v>4</v>
       </c>
       <c r="D30">
-        <v>2181</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>6492</v>
+        <v>8673.000000013044</v>
       </c>
       <c r="F30" s="1">
-        <v>0.02990605435909073</v>
+        <v>0.03995305136426124</v>
       </c>
       <c r="G30">
         <v>2181.697</v>
@@ -1112,13 +1112,13 @@
         <v>4</v>
       </c>
       <c r="D31">
-        <v>2181</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>8673</v>
+        <v>8673.000000013044</v>
       </c>
       <c r="F31" s="1">
-        <v>0.03995305136420115</v>
+        <v>0.03995305136426124</v>
       </c>
       <c r="G31">
         <v>2181.697</v>
@@ -1138,10 +1138,10 @@
         <v>2181</v>
       </c>
       <c r="E32">
-        <v>10854</v>
+        <v>10854.00000001304</v>
       </c>
       <c r="F32" s="1">
-        <v>0.05000004836931158</v>
+        <v>0.05000004836937166</v>
       </c>
       <c r="G32">
         <v>2181.697</v>
@@ -1158,13 +1158,13 @@
         <v>5</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>2181</v>
       </c>
       <c r="E33">
-        <v>10854</v>
+        <v>13035.00000001304</v>
       </c>
       <c r="F33" s="1">
-        <v>0.05000004836931158</v>
+        <v>0.06004704537448209</v>
       </c>
       <c r="G33">
         <v>2181.697</v>
@@ -1181,13 +1181,13 @@
         <v>5</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>2180.999999991052</v>
       </c>
       <c r="E34">
-        <v>10854</v>
+        <v>15216.0000000041</v>
       </c>
       <c r="F34" s="1">
-        <v>0.05000004836931158</v>
+        <v>0.0700940423795513</v>
       </c>
       <c r="G34">
         <v>2181.697</v>
@@ -1204,13 +1204,13 @@
         <v>5</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>2181</v>
       </c>
       <c r="E35">
-        <v>10854</v>
+        <v>17397.0000000041</v>
       </c>
       <c r="F35" s="1">
-        <v>0.05000004836931158</v>
+        <v>0.08014103938466172</v>
       </c>
       <c r="G35">
         <v>2181.697</v>
@@ -1227,13 +1227,13 @@
         <v>5</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>2181</v>
       </c>
       <c r="E36">
-        <v>10854</v>
+        <v>19578.0000000041</v>
       </c>
       <c r="F36" s="1">
-        <v>0.05000004836931158</v>
+        <v>0.09018803638977214</v>
       </c>
       <c r="G36">
         <v>2181.697</v>
@@ -1250,13 +1250,13 @@
         <v>5</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>2181</v>
       </c>
       <c r="E37">
-        <v>10854</v>
+        <v>21759.0000000041</v>
       </c>
       <c r="F37" s="1">
-        <v>0.05000004836931158</v>
+        <v>0.1002350333948826</v>
       </c>
       <c r="G37">
         <v>2181.697</v>
@@ -1273,13 +1273,13 @@
         <v>5</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>2181</v>
       </c>
       <c r="E38">
-        <v>10854</v>
+        <v>23940.0000000041</v>
       </c>
       <c r="F38" s="1">
-        <v>0.05000004836931158</v>
+        <v>0.110282030399993</v>
       </c>
       <c r="G38">
         <v>2181.697</v>
@@ -1296,13 +1296,13 @@
         <v>5</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>2181</v>
       </c>
       <c r="E39">
-        <v>10854</v>
+        <v>26121.0000000041</v>
       </c>
       <c r="F39" s="1">
-        <v>0.05000004836931158</v>
+        <v>0.1203290274051034</v>
       </c>
       <c r="G39">
         <v>2181.697</v>
@@ -1319,13 +1319,13 @@
         <v>5</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>2180.999999999978</v>
       </c>
       <c r="E40">
-        <v>10854</v>
+        <v>28302.00000000407</v>
       </c>
       <c r="F40" s="1">
-        <v>0.05000004836931158</v>
+        <v>0.1303760244102137</v>
       </c>
       <c r="G40">
         <v>2181.697</v>
@@ -1342,13 +1342,13 @@
         <v>5</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>2180.999999995409</v>
       </c>
       <c r="E41">
-        <v>10854</v>
+        <v>30482.99999999948</v>
       </c>
       <c r="F41" s="1">
-        <v>0.05000004836931158</v>
+        <v>0.140423021415303</v>
       </c>
       <c r="G41">
         <v>2181.697</v>
@@ -1365,13 +1365,13 @@
         <v>5</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>2181</v>
       </c>
       <c r="E42">
-        <v>10854</v>
+        <v>32663.99999999948</v>
       </c>
       <c r="F42" s="1">
-        <v>0.05000004836931158</v>
+        <v>0.1504700184204134</v>
       </c>
       <c r="G42">
         <v>2181.697</v>
@@ -1391,10 +1391,10 @@
         <v>2181</v>
       </c>
       <c r="E43">
-        <v>13035</v>
+        <v>34844.99999999948</v>
       </c>
       <c r="F43" s="1">
-        <v>0.060047045374422</v>
+        <v>0.1605170154255239</v>
       </c>
       <c r="G43">
         <v>2181.697</v>
@@ -1411,13 +1411,13 @@
         <v>5</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>2181</v>
       </c>
       <c r="E44">
-        <v>13035</v>
+        <v>37025.99999999948</v>
       </c>
       <c r="F44" s="1">
-        <v>0.060047045374422</v>
+        <v>0.1705640124306343</v>
       </c>
       <c r="G44">
         <v>2181.697</v>
@@ -1434,13 +1434,13 @@
         <v>5</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>2181</v>
       </c>
       <c r="E45">
-        <v>13035</v>
+        <v>39206.99999999948</v>
       </c>
       <c r="F45" s="1">
-        <v>0.060047045374422</v>
+        <v>0.1806110094357447</v>
       </c>
       <c r="G45">
         <v>2181.697</v>
@@ -1457,13 +1457,13 @@
         <v>5</v>
       </c>
       <c r="D46">
-        <v>2150</v>
+        <v>2181</v>
       </c>
       <c r="E46">
-        <v>15185</v>
+        <v>41387.99999999948</v>
       </c>
       <c r="F46" s="1">
-        <v>0.06995123774534699</v>
+        <v>0.1906580064408551</v>
       </c>
       <c r="G46">
         <v>2181.697</v>
@@ -1483,10 +1483,10 @@
         <v>2181</v>
       </c>
       <c r="E47">
-        <v>17366</v>
+        <v>43568.99999999948</v>
       </c>
       <c r="F47" s="1">
-        <v>0.07999823475045742</v>
+        <v>0.2007050034459656</v>
       </c>
       <c r="G47">
         <v>2181.697</v>
@@ -1503,13 +1503,13 @@
         <v>5</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>2181</v>
       </c>
       <c r="E48">
-        <v>17366</v>
+        <v>45749.99999999948</v>
       </c>
       <c r="F48" s="1">
-        <v>0.07999823475045742</v>
+        <v>0.210752000451076</v>
       </c>
       <c r="G48">
         <v>2181.697</v>
@@ -1529,10 +1529,10 @@
         <v>2181</v>
       </c>
       <c r="E49">
-        <v>19547</v>
+        <v>47930.99999999948</v>
       </c>
       <c r="F49" s="1">
-        <v>0.09004523175556785</v>
+        <v>0.2207989974561864</v>
       </c>
       <c r="G49">
         <v>2181.697</v>
@@ -1552,10 +1552,10 @@
         <v>2181</v>
       </c>
       <c r="E50">
-        <v>21728</v>
+        <v>50111.99999999948</v>
       </c>
       <c r="F50" s="1">
-        <v>0.1000922287606783</v>
+        <v>0.2308459944612968</v>
       </c>
       <c r="G50">
         <v>2181.697</v>
@@ -1572,13 +1572,13 @@
         <v>5</v>
       </c>
       <c r="D51">
-        <v>2181</v>
+        <v>2180.999999996677</v>
       </c>
       <c r="E51">
-        <v>23909</v>
+        <v>52292.99999999616</v>
       </c>
       <c r="F51" s="1">
-        <v>0.1101392257657887</v>
+        <v>0.240892991466392</v>
       </c>
       <c r="G51">
         <v>2181.697</v>
@@ -1595,13 +1595,13 @@
         <v>5</v>
       </c>
       <c r="D52">
-        <v>2140</v>
+        <v>2181</v>
       </c>
       <c r="E52">
-        <v>26049</v>
+        <v>54473.99999999616</v>
       </c>
       <c r="F52" s="1">
-        <v>0.1199973521256861</v>
+        <v>0.2509399884715024</v>
       </c>
       <c r="G52">
         <v>2181.697</v>
@@ -1621,10 +1621,10 @@
         <v>2181</v>
       </c>
       <c r="E53">
-        <v>28230</v>
+        <v>56654.99999999616</v>
       </c>
       <c r="F53" s="1">
-        <v>0.1300443491307965</v>
+        <v>0.2609869854766128</v>
       </c>
       <c r="G53">
         <v>2181.697</v>
@@ -1644,10 +1644,10 @@
         <v>2181</v>
       </c>
       <c r="E54">
-        <v>30411</v>
+        <v>58835.99999999616</v>
       </c>
       <c r="F54" s="1">
-        <v>0.140091346135907</v>
+        <v>0.2710339824817232</v>
       </c>
       <c r="G54">
         <v>2181.697</v>
@@ -1667,10 +1667,10 @@
         <v>2181</v>
       </c>
       <c r="E55">
-        <v>32592</v>
+        <v>61016.99999999616</v>
       </c>
       <c r="F55" s="1">
-        <v>0.1501383431410174</v>
+        <v>0.2810809794868336</v>
       </c>
       <c r="G55">
         <v>2181.697</v>
@@ -1690,10 +1690,10 @@
         <v>2181</v>
       </c>
       <c r="E56">
-        <v>34773</v>
+        <v>63197.99999999616</v>
       </c>
       <c r="F56" s="1">
-        <v>0.1601853401461278</v>
+        <v>0.2911279764919441</v>
       </c>
       <c r="G56">
         <v>2181.697</v>
@@ -1713,10 +1713,10 @@
         <v>2181</v>
       </c>
       <c r="E57">
-        <v>36954</v>
+        <v>65378.99999999616</v>
       </c>
       <c r="F57" s="1">
-        <v>0.1702323371512383</v>
+        <v>0.3011749734970545</v>
       </c>
       <c r="G57">
         <v>2181.697</v>
@@ -1736,10 +1736,10 @@
         <v>2181</v>
       </c>
       <c r="E58">
-        <v>39135</v>
+        <v>67559.99999999616</v>
       </c>
       <c r="F58" s="1">
-        <v>0.1802793341563487</v>
+        <v>0.3112219705021649</v>
       </c>
       <c r="G58">
         <v>2181.697</v>
@@ -1756,13 +1756,13 @@
         <v>5</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>2181</v>
       </c>
       <c r="E59">
-        <v>39135</v>
+        <v>69740.99999999616</v>
       </c>
       <c r="F59" s="1">
-        <v>0.1802793341563487</v>
+        <v>0.3212689675072753</v>
       </c>
       <c r="G59">
         <v>2181.697</v>
@@ -1779,13 +1779,13 @@
         <v>5</v>
       </c>
       <c r="D60">
-        <v>1477</v>
+        <v>2180.999999985142</v>
       </c>
       <c r="E60">
-        <v>40612</v>
+        <v>71921.9999999813</v>
       </c>
       <c r="F60" s="1">
-        <v>0.187083283985119</v>
+        <v>0.3313159645123173</v>
       </c>
       <c r="G60">
         <v>2181.697</v>
@@ -1802,13 +1802,13 @@
         <v>5</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>2181</v>
       </c>
       <c r="E61">
-        <v>40612</v>
+        <v>74102.9999999813</v>
       </c>
       <c r="F61" s="1">
-        <v>0.187083283985119</v>
+        <v>0.3413629615174277</v>
       </c>
       <c r="G61">
         <v>2181.697</v>
@@ -1828,10 +1828,10 @@
         <v>2181</v>
       </c>
       <c r="E62">
-        <v>42793</v>
+        <v>76283.9999999813</v>
       </c>
       <c r="F62" s="1">
-        <v>0.1971302809902294</v>
+        <v>0.3514099585225382</v>
       </c>
       <c r="G62">
         <v>2181.697</v>
@@ -1851,10 +1851,10 @@
         <v>2181</v>
       </c>
       <c r="E63">
-        <v>44974</v>
+        <v>78464.9999999813</v>
       </c>
       <c r="F63" s="1">
-        <v>0.2071772779953399</v>
+        <v>0.3614569555276486</v>
       </c>
       <c r="G63">
         <v>2181.697</v>
@@ -1874,10 +1874,10 @@
         <v>2181</v>
       </c>
       <c r="E64">
-        <v>47155</v>
+        <v>80645.9999999813</v>
       </c>
       <c r="F64" s="1">
-        <v>0.2172242750004503</v>
+        <v>0.371503952532759</v>
       </c>
       <c r="G64">
         <v>2181.697</v>
@@ -1897,10 +1897,10 @@
         <v>2181</v>
       </c>
       <c r="E65">
-        <v>49336</v>
+        <v>82826.9999999813</v>
       </c>
       <c r="F65" s="1">
-        <v>0.2272712720055607</v>
+        <v>0.3815509495378694</v>
       </c>
       <c r="G65">
         <v>2181.697</v>
@@ -1920,10 +1920,10 @@
         <v>2181</v>
       </c>
       <c r="E66">
-        <v>51517</v>
+        <v>85007.9999999813</v>
       </c>
       <c r="F66" s="1">
-        <v>0.2373182690106711</v>
+        <v>0.3915979465429799</v>
       </c>
       <c r="G66">
         <v>2181.697</v>
@@ -1943,10 +1943,10 @@
         <v>2181</v>
       </c>
       <c r="E67">
-        <v>53698</v>
+        <v>87188.9999999813</v>
       </c>
       <c r="F67" s="1">
-        <v>0.2473652660157816</v>
+        <v>0.4016449435480903</v>
       </c>
       <c r="G67">
         <v>2181.697</v>
@@ -1966,10 +1966,10 @@
         <v>2181</v>
       </c>
       <c r="E68">
-        <v>55879</v>
+        <v>89369.9999999813</v>
       </c>
       <c r="F68" s="1">
-        <v>0.257412263020892</v>
+        <v>0.4116919405532007</v>
       </c>
       <c r="G68">
         <v>2181.697</v>
@@ -1989,10 +1989,10 @@
         <v>2181</v>
       </c>
       <c r="E69">
-        <v>58060</v>
+        <v>91550.9999999813</v>
       </c>
       <c r="F69" s="1">
-        <v>0.2674592600260024</v>
+        <v>0.4217389375583112</v>
       </c>
       <c r="G69">
         <v>2181.697</v>
@@ -2012,10 +2012,10 @@
         <v>2181</v>
       </c>
       <c r="E70">
-        <v>60241</v>
+        <v>93731.9999999813</v>
       </c>
       <c r="F70" s="1">
-        <v>0.2775062570311128</v>
+        <v>0.4317859345634216</v>
       </c>
       <c r="G70">
         <v>2181.697</v>
@@ -2035,10 +2035,10 @@
         <v>2181</v>
       </c>
       <c r="E71">
-        <v>62422</v>
+        <v>95912.9999999813</v>
       </c>
       <c r="F71" s="1">
-        <v>0.2875532540362233</v>
+        <v>0.441832931568532</v>
       </c>
       <c r="G71">
         <v>2181.697</v>
@@ -2058,10 +2058,10 @@
         <v>2181</v>
       </c>
       <c r="E72">
-        <v>64603</v>
+        <v>98093.9999999813</v>
       </c>
       <c r="F72" s="1">
-        <v>0.2976002510413337</v>
+        <v>0.4518799285736424</v>
       </c>
       <c r="G72">
         <v>2181.697</v>
@@ -2081,10 +2081,10 @@
         <v>2181</v>
       </c>
       <c r="E73">
-        <v>66784</v>
+        <v>100274.9999999813</v>
       </c>
       <c r="F73" s="1">
-        <v>0.3076472480464441</v>
+        <v>0.4619269255787529</v>
       </c>
       <c r="G73">
         <v>2181.697</v>
@@ -2104,10 +2104,10 @@
         <v>2181</v>
       </c>
       <c r="E74">
-        <v>68965</v>
+        <v>102455.9999999813</v>
       </c>
       <c r="F74" s="1">
-        <v>0.3176942450515545</v>
+        <v>0.4719739225838633</v>
       </c>
       <c r="G74">
         <v>2181.697</v>
@@ -2127,10 +2127,10 @@
         <v>2181</v>
       </c>
       <c r="E75">
-        <v>71146</v>
+        <v>104636.9999999813</v>
       </c>
       <c r="F75" s="1">
-        <v>0.3277412420566649</v>
+        <v>0.4820209195889737</v>
       </c>
       <c r="G75">
         <v>2181.697</v>
@@ -2150,10 +2150,10 @@
         <v>2181</v>
       </c>
       <c r="E76">
-        <v>73327</v>
+        <v>106817.9999999813</v>
       </c>
       <c r="F76" s="1">
-        <v>0.3377882390617754</v>
+        <v>0.4920679165940841</v>
       </c>
       <c r="G76">
         <v>2181.697</v>
@@ -2173,10 +2173,10 @@
         <v>2181</v>
       </c>
       <c r="E77">
-        <v>75508</v>
+        <v>108998.9999999813</v>
       </c>
       <c r="F77" s="1">
-        <v>0.3478352360668858</v>
+        <v>0.5021149135991946</v>
       </c>
       <c r="G77">
         <v>2181.697</v>
@@ -2196,10 +2196,10 @@
         <v>2181</v>
       </c>
       <c r="E78">
-        <v>77689</v>
+        <v>111179.9999999813</v>
       </c>
       <c r="F78" s="1">
-        <v>0.3578822330719962</v>
+        <v>0.512161910604305</v>
       </c>
       <c r="G78">
         <v>2181.697</v>
@@ -2219,10 +2219,10 @@
         <v>2181</v>
       </c>
       <c r="E79">
-        <v>79870</v>
+        <v>113360.9999999813</v>
       </c>
       <c r="F79" s="1">
-        <v>0.3679292300771067</v>
+        <v>0.5222089076094155</v>
       </c>
       <c r="G79">
         <v>2181.697</v>
@@ -2242,10 +2242,10 @@
         <v>2181</v>
       </c>
       <c r="E80">
-        <v>82051</v>
+        <v>115541.9999999813</v>
       </c>
       <c r="F80" s="1">
-        <v>0.3779762270822171</v>
+        <v>0.5322559046145259</v>
       </c>
       <c r="G80">
         <v>2181.697</v>
@@ -2265,10 +2265,10 @@
         <v>2181</v>
       </c>
       <c r="E81">
-        <v>84232</v>
+        <v>117722.9999999813</v>
       </c>
       <c r="F81" s="1">
-        <v>0.3880232240873275</v>
+        <v>0.5423029016196363</v>
       </c>
       <c r="G81">
         <v>2181.697</v>
@@ -2288,10 +2288,10 @@
         <v>2181</v>
       </c>
       <c r="E82">
-        <v>86413</v>
+        <v>119903.9999999813</v>
       </c>
       <c r="F82" s="1">
-        <v>0.3980702210924379</v>
+        <v>0.5523498986247467</v>
       </c>
       <c r="G82">
         <v>2181.697</v>
@@ -2311,10 +2311,10 @@
         <v>2181</v>
       </c>
       <c r="E83">
-        <v>88594</v>
+        <v>122084.9999999813</v>
       </c>
       <c r="F83" s="1">
-        <v>0.4081172180975484</v>
+        <v>0.5623968956298572</v>
       </c>
       <c r="G83">
         <v>2181.697</v>
@@ -2334,10 +2334,10 @@
         <v>2181</v>
       </c>
       <c r="E84">
-        <v>90775</v>
+        <v>124265.9999999813</v>
       </c>
       <c r="F84" s="1">
-        <v>0.4181642151026588</v>
+        <v>0.5724438926349675</v>
       </c>
       <c r="G84">
         <v>2181.697</v>
@@ -2357,10 +2357,10 @@
         <v>2181</v>
       </c>
       <c r="E85">
-        <v>92956</v>
+        <v>126446.9999999813</v>
       </c>
       <c r="F85" s="1">
-        <v>0.4282112121077692</v>
+        <v>0.582490889640078</v>
       </c>
       <c r="G85">
         <v>2181.697</v>
@@ -2380,10 +2380,10 @@
         <v>2181</v>
       </c>
       <c r="E86">
-        <v>95137</v>
+        <v>128627.9999999813</v>
       </c>
       <c r="F86" s="1">
-        <v>0.4382582091128796</v>
+        <v>0.5925378866451885</v>
       </c>
       <c r="G86">
         <v>2181.697</v>
@@ -2403,10 +2403,10 @@
         <v>2181</v>
       </c>
       <c r="E87">
-        <v>97318</v>
+        <v>130808.9999999813</v>
       </c>
       <c r="F87" s="1">
-        <v>0.4483052061179901</v>
+        <v>0.6025848836502988</v>
       </c>
       <c r="G87">
         <v>2181.697</v>
@@ -2426,10 +2426,10 @@
         <v>2181</v>
       </c>
       <c r="E88">
-        <v>99499</v>
+        <v>132989.9999999813</v>
       </c>
       <c r="F88" s="1">
-        <v>0.4583522031231005</v>
+        <v>0.6126318806554093</v>
       </c>
       <c r="G88">
         <v>2181.697</v>
@@ -2449,10 +2449,10 @@
         <v>2181</v>
       </c>
       <c r="E89">
-        <v>101680</v>
+        <v>135170.9999999813</v>
       </c>
       <c r="F89" s="1">
-        <v>0.4683992001282109</v>
+        <v>0.6226788776605197</v>
       </c>
       <c r="G89">
         <v>2181.697</v>
@@ -2472,10 +2472,10 @@
         <v>2181</v>
       </c>
       <c r="E90">
-        <v>103861</v>
+        <v>137351.9999999813</v>
       </c>
       <c r="F90" s="1">
-        <v>0.4784461971333213</v>
+        <v>0.6327258746656301</v>
       </c>
       <c r="G90">
         <v>2181.697</v>
@@ -2495,10 +2495,10 @@
         <v>2181</v>
       </c>
       <c r="E91">
-        <v>106042</v>
+        <v>139532.9999999813</v>
       </c>
       <c r="F91" s="1">
-        <v>0.4884931941384317</v>
+        <v>0.6427728716707406</v>
       </c>
       <c r="G91">
         <v>2181.697</v>
@@ -2518,10 +2518,10 @@
         <v>2181</v>
       </c>
       <c r="E92">
-        <v>108223</v>
+        <v>141713.9999999813</v>
       </c>
       <c r="F92" s="1">
-        <v>0.4985401911435422</v>
+        <v>0.652819868675851</v>
       </c>
       <c r="G92">
         <v>2181.697</v>
@@ -2541,10 +2541,10 @@
         <v>2181</v>
       </c>
       <c r="E93">
-        <v>110404</v>
+        <v>143894.9999999813</v>
       </c>
       <c r="F93" s="1">
-        <v>0.5085871881486526</v>
+        <v>0.6628668656809614</v>
       </c>
       <c r="G93">
         <v>2181.697</v>
@@ -2564,10 +2564,10 @@
         <v>2181</v>
       </c>
       <c r="E94">
-        <v>112585</v>
+        <v>146075.9999999813</v>
       </c>
       <c r="F94" s="1">
-        <v>0.518634185153763</v>
+        <v>0.6729138626860718</v>
       </c>
       <c r="G94">
         <v>2181.697</v>
@@ -2587,10 +2587,10 @@
         <v>2181</v>
       </c>
       <c r="E95">
-        <v>114766</v>
+        <v>148256.9999999813</v>
       </c>
       <c r="F95" s="1">
-        <v>0.5286811821588735</v>
+        <v>0.6829608596911823</v>
       </c>
       <c r="G95">
         <v>2181.697</v>
@@ -2610,10 +2610,10 @@
         <v>2181</v>
       </c>
       <c r="E96">
-        <v>116947</v>
+        <v>150437.9999999813</v>
       </c>
       <c r="F96" s="1">
-        <v>0.5387281791639839</v>
+        <v>0.6930078566962927</v>
       </c>
       <c r="G96">
         <v>2181.697</v>
@@ -2633,10 +2633,10 @@
         <v>2181</v>
       </c>
       <c r="E97">
-        <v>119128</v>
+        <v>152618.9999999813</v>
       </c>
       <c r="F97" s="1">
-        <v>0.5487751761690943</v>
+        <v>0.7030548537014031</v>
       </c>
       <c r="G97">
         <v>2181.697</v>
@@ -2656,10 +2656,10 @@
         <v>2181</v>
       </c>
       <c r="E98">
-        <v>121309</v>
+        <v>154799.9999999813</v>
       </c>
       <c r="F98" s="1">
-        <v>0.5588221731742047</v>
+        <v>0.7131018507065136</v>
       </c>
       <c r="G98">
         <v>2181.697</v>
@@ -2679,10 +2679,10 @@
         <v>2181</v>
       </c>
       <c r="E99">
-        <v>123490</v>
+        <v>156980.9999999813</v>
       </c>
       <c r="F99" s="1">
-        <v>0.5688691701793152</v>
+        <v>0.7231488477116239</v>
       </c>
       <c r="G99">
         <v>2181.697</v>
@@ -2702,10 +2702,10 @@
         <v>2181</v>
       </c>
       <c r="E100">
-        <v>125671</v>
+        <v>159161.9999999813</v>
       </c>
       <c r="F100" s="1">
-        <v>0.5789161671844256</v>
+        <v>0.7331958447167344</v>
       </c>
       <c r="G100">
         <v>2181.697</v>
@@ -2725,10 +2725,10 @@
         <v>2181</v>
       </c>
       <c r="E101">
-        <v>127852</v>
+        <v>161342.9999999813</v>
       </c>
       <c r="F101" s="1">
-        <v>0.588963164189536</v>
+        <v>0.7432428417218448</v>
       </c>
       <c r="G101">
         <v>2181.697</v>
@@ -2748,10 +2748,10 @@
         <v>2181</v>
       </c>
       <c r="E102">
-        <v>130033</v>
+        <v>163523.9999999813</v>
       </c>
       <c r="F102" s="1">
-        <v>0.5990101611946465</v>
+        <v>0.7532898387269552</v>
       </c>
       <c r="G102">
         <v>2181.697</v>
@@ -2771,10 +2771,10 @@
         <v>2181</v>
       </c>
       <c r="E103">
-        <v>132214</v>
+        <v>165704.9999999813</v>
       </c>
       <c r="F103" s="1">
-        <v>0.6090571581997568</v>
+        <v>0.7633368357320657</v>
       </c>
       <c r="G103">
         <v>2181.697</v>
@@ -2794,10 +2794,10 @@
         <v>2181</v>
       </c>
       <c r="E104">
-        <v>134395</v>
+        <v>167885.9999999813</v>
       </c>
       <c r="F104" s="1">
-        <v>0.6191041552048673</v>
+        <v>0.773383832737176</v>
       </c>
       <c r="G104">
         <v>2181.697</v>
@@ -2817,10 +2817,10 @@
         <v>2181</v>
       </c>
       <c r="E105">
-        <v>136576</v>
+        <v>170066.9999999813</v>
       </c>
       <c r="F105" s="1">
-        <v>0.6291511522099777</v>
+        <v>0.7834308297422865</v>
       </c>
       <c r="G105">
         <v>2181.697</v>
@@ -2840,10 +2840,10 @@
         <v>2181</v>
       </c>
       <c r="E106">
-        <v>138757</v>
+        <v>172247.9999999813</v>
       </c>
       <c r="F106" s="1">
-        <v>0.6391981492150881</v>
+        <v>0.793477826747397</v>
       </c>
       <c r="G106">
         <v>2181.697</v>
@@ -2863,10 +2863,10 @@
         <v>2181</v>
       </c>
       <c r="E107">
-        <v>140938</v>
+        <v>174428.9999999813</v>
       </c>
       <c r="F107" s="1">
-        <v>0.6492451462201986</v>
+        <v>0.8035248237525073</v>
       </c>
       <c r="G107">
         <v>2181.697</v>
@@ -2883,16 +2883,16 @@
         <v>7</v>
       </c>
       <c r="D108">
-        <v>2181</v>
+        <v>2109</v>
       </c>
       <c r="E108">
-        <v>143119</v>
+        <v>176537.9999999813</v>
       </c>
       <c r="F108" s="1">
-        <v>0.6592921432253089</v>
+        <v>0.8132401454782193</v>
       </c>
       <c r="G108">
-        <v>2181.697</v>
+        <v>2109.30829354</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -2906,16 +2906,16 @@
         <v>7</v>
       </c>
       <c r="D109">
-        <v>2181</v>
+        <v>2109</v>
       </c>
       <c r="E109">
-        <v>145300</v>
+        <v>178646.9999999813</v>
       </c>
       <c r="F109" s="1">
-        <v>0.6693391402304194</v>
+        <v>0.8229554672039314</v>
       </c>
       <c r="G109">
-        <v>2181.697</v>
+        <v>2109.30829354</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -2929,16 +2929,16 @@
         <v>7</v>
       </c>
       <c r="D110">
-        <v>2181</v>
+        <v>2109</v>
       </c>
       <c r="E110">
-        <v>147481</v>
+        <v>180755.9999999813</v>
       </c>
       <c r="F110" s="1">
-        <v>0.6793861372355299</v>
+        <v>0.8326707889296434</v>
       </c>
       <c r="G110">
-        <v>2181.697</v>
+        <v>2109.30829354</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -2952,16 +2952,16 @@
         <v>7</v>
       </c>
       <c r="D111">
-        <v>2181</v>
+        <v>2012</v>
       </c>
       <c r="E111">
-        <v>149662</v>
+        <v>182767.9999999813</v>
       </c>
       <c r="F111" s="1">
-        <v>0.6894331342406402</v>
+        <v>0.8419392703483881</v>
       </c>
       <c r="G111">
-        <v>2181.697</v>
+        <v>2012.79001826</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -2975,16 +2975,16 @@
         <v>7</v>
       </c>
       <c r="D112">
-        <v>2181</v>
+        <v>2012</v>
       </c>
       <c r="E112">
-        <v>151843</v>
+        <v>184779.9999999813</v>
       </c>
       <c r="F112" s="1">
-        <v>0.6994801312457507</v>
+        <v>0.8512077517671328</v>
       </c>
       <c r="G112">
-        <v>2181.697</v>
+        <v>2012.79001826</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -2998,16 +2998,16 @@
         <v>7</v>
       </c>
       <c r="D113">
-        <v>2181</v>
+        <v>2012</v>
       </c>
       <c r="E113">
-        <v>154024</v>
+        <v>186791.9999999813</v>
       </c>
       <c r="F113" s="1">
-        <v>0.7095271282508611</v>
+        <v>0.8604762331858774</v>
       </c>
       <c r="G113">
-        <v>2181.697</v>
+        <v>2012.79001826</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -3021,16 +3021,16 @@
         <v>7</v>
       </c>
       <c r="D114">
-        <v>2181</v>
+        <v>2012</v>
       </c>
       <c r="E114">
-        <v>156205</v>
+        <v>188803.9999999813</v>
       </c>
       <c r="F114" s="1">
-        <v>0.7195741252559715</v>
+        <v>0.8697447146046221</v>
       </c>
       <c r="G114">
-        <v>2181.697</v>
+        <v>2012.79001826</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -3044,16 +3044,16 @@
         <v>7</v>
       </c>
       <c r="D115">
-        <v>2181</v>
+        <v>2012</v>
       </c>
       <c r="E115">
-        <v>158386</v>
+        <v>190815.9999999813</v>
       </c>
       <c r="F115" s="1">
-        <v>0.729621122261082</v>
+        <v>0.8790131960233668</v>
       </c>
       <c r="G115">
-        <v>2181.697</v>
+        <v>2012.79001826</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -3067,16 +3067,16 @@
         <v>7</v>
       </c>
       <c r="D116">
-        <v>2181</v>
+        <v>1916</v>
       </c>
       <c r="E116">
-        <v>160567</v>
+        <v>192731.9999999813</v>
       </c>
       <c r="F116" s="1">
-        <v>0.7396681192661924</v>
+        <v>0.887839443736247</v>
       </c>
       <c r="G116">
-        <v>2181.697</v>
+        <v>1916.27174298</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -3090,16 +3090,16 @@
         <v>7</v>
       </c>
       <c r="D117">
-        <v>2181</v>
+        <v>1916</v>
       </c>
       <c r="E117">
-        <v>162748</v>
+        <v>194647.9999999813</v>
       </c>
       <c r="F117" s="1">
-        <v>0.7497151162713028</v>
+        <v>0.8966656914491271</v>
       </c>
       <c r="G117">
-        <v>2181.697</v>
+        <v>1916.27174298</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -3113,16 +3113,16 @@
         <v>7</v>
       </c>
       <c r="D118">
-        <v>2181</v>
+        <v>1916</v>
       </c>
       <c r="E118">
-        <v>164929</v>
+        <v>196563.9999999813</v>
       </c>
       <c r="F118" s="1">
-        <v>0.7597621132764132</v>
+        <v>0.9054919391620072</v>
       </c>
       <c r="G118">
-        <v>2181.697</v>
+        <v>1916.27174298</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -3136,16 +3136,16 @@
         <v>7</v>
       </c>
       <c r="D119">
-        <v>2181</v>
+        <v>1916</v>
       </c>
       <c r="E119">
-        <v>167110</v>
+        <v>198479.9999999813</v>
       </c>
       <c r="F119" s="1">
-        <v>0.7698091102815237</v>
+        <v>0.9143181868748874</v>
       </c>
       <c r="G119">
-        <v>2181.697</v>
+        <v>1916.27174298</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -3159,16 +3159,16 @@
         <v>7</v>
       </c>
       <c r="D120">
-        <v>2181</v>
+        <v>1819</v>
       </c>
       <c r="E120">
-        <v>169291</v>
+        <v>200298.9999999813</v>
       </c>
       <c r="F120" s="1">
-        <v>0.779856107286634</v>
+        <v>0.9226975942808002</v>
       </c>
       <c r="G120">
-        <v>2181.697</v>
+        <v>1819.7534677</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -3182,16 +3182,16 @@
         <v>7</v>
       </c>
       <c r="D121">
-        <v>2181</v>
+        <v>1819</v>
       </c>
       <c r="E121">
-        <v>171472</v>
+        <v>202117.9999999813</v>
       </c>
       <c r="F121" s="1">
-        <v>0.7899031042917445</v>
+        <v>0.931077001686713</v>
       </c>
       <c r="G121">
-        <v>2181.697</v>
+        <v>1819.7534677</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -3205,16 +3205,16 @@
         <v>7</v>
       </c>
       <c r="D122">
-        <v>2181</v>
+        <v>1819</v>
       </c>
       <c r="E122">
-        <v>173653</v>
+        <v>203936.9999999813</v>
       </c>
       <c r="F122" s="1">
-        <v>0.799950101296855</v>
+        <v>0.9394564090926258</v>
       </c>
       <c r="G122">
-        <v>2181.697</v>
+        <v>1819.7534677</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -3228,16 +3228,16 @@
         <v>7</v>
       </c>
       <c r="D123">
-        <v>2181</v>
+        <v>1819</v>
       </c>
       <c r="E123">
-        <v>175834</v>
+        <v>205755.9999999813</v>
       </c>
       <c r="F123" s="1">
-        <v>0.8099970983019653</v>
+        <v>0.9478358164985387</v>
       </c>
       <c r="G123">
-        <v>2181.697</v>
+        <v>1819.7534677</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -3251,16 +3251,16 @@
         <v>8</v>
       </c>
       <c r="D124">
-        <v>0</v>
+        <v>919</v>
       </c>
       <c r="E124">
-        <v>175834</v>
+        <v>206674.9999999813</v>
       </c>
       <c r="F124" s="1">
-        <v>0.8099970983019653</v>
+        <v>0.9520692829119712</v>
       </c>
       <c r="G124">
-        <v>2181.697</v>
+        <v>1819.7534677</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -3277,13 +3277,13 @@
         <v>0</v>
       </c>
       <c r="E125">
-        <v>175834</v>
+        <v>206674.9999999813</v>
       </c>
       <c r="F125" s="1">
-        <v>0.8099970983019653</v>
+        <v>0.9520692829119712</v>
       </c>
       <c r="G125">
-        <v>2181.697</v>
+        <v>1819.7534677</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -3300,13 +3300,13 @@
         <v>0</v>
       </c>
       <c r="E126">
-        <v>175834</v>
+        <v>206674.9999999813</v>
       </c>
       <c r="F126" s="1">
-        <v>0.8099970983019653</v>
+        <v>0.9520692829119712</v>
       </c>
       <c r="G126">
-        <v>2181.697</v>
+        <v>1819.7534677</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -3323,13 +3323,13 @@
         <v>0</v>
       </c>
       <c r="E127">
-        <v>175834</v>
+        <v>206674.9999999813</v>
       </c>
       <c r="F127" s="1">
-        <v>0.8099970983019653</v>
+        <v>0.9520692829119712</v>
       </c>
       <c r="G127">
-        <v>2181.697</v>
+        <v>1819.7534677</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -3346,13 +3346,13 @@
         <v>0</v>
       </c>
       <c r="E128">
-        <v>175834</v>
+        <v>206674.9999999813</v>
       </c>
       <c r="F128" s="1">
-        <v>0.8099970983019653</v>
+        <v>0.9520692829119712</v>
       </c>
       <c r="G128">
-        <v>2181.697</v>
+        <v>1819.7534677</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -3366,16 +3366,16 @@
         <v>8</v>
       </c>
       <c r="D129">
-        <v>2109</v>
+        <v>0</v>
       </c>
       <c r="E129">
-        <v>177943</v>
+        <v>206674.9999999813</v>
       </c>
       <c r="F129" s="1">
-        <v>0.8197124200276773</v>
+        <v>0.9520692829119712</v>
       </c>
       <c r="G129">
-        <v>2109.30829354</v>
+        <v>1819.7534677</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -3389,16 +3389,16 @@
         <v>8</v>
       </c>
       <c r="D130">
-        <v>2109</v>
+        <v>0</v>
       </c>
       <c r="E130">
-        <v>180052</v>
+        <v>206674.9999999813</v>
       </c>
       <c r="F130" s="1">
-        <v>0.8294277417533894</v>
+        <v>0.9520692829119712</v>
       </c>
       <c r="G130">
-        <v>2109.30829354</v>
+        <v>1819.7534677</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -3412,16 +3412,16 @@
         <v>8</v>
       </c>
       <c r="D131">
-        <v>2109</v>
+        <v>0</v>
       </c>
       <c r="E131">
-        <v>182161</v>
+        <v>206674.9999999813</v>
       </c>
       <c r="F131" s="1">
-        <v>0.8391430634791014</v>
+        <v>0.9520692829119712</v>
       </c>
       <c r="G131">
-        <v>2109.30829354</v>
+        <v>1819.7534677</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -3435,16 +3435,16 @@
         <v>8</v>
       </c>
       <c r="D132">
-        <v>0</v>
+        <v>1722</v>
       </c>
       <c r="E132">
-        <v>182161</v>
+        <v>208396.9999999813</v>
       </c>
       <c r="F132" s="1">
-        <v>0.8391430634791014</v>
+        <v>0.9600018500109168</v>
       </c>
       <c r="G132">
-        <v>2109.30829354</v>
+        <v>1722.58068332</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -3461,13 +3461,13 @@
         <v>0</v>
       </c>
       <c r="E133">
-        <v>182161</v>
+        <v>208396.9999999813</v>
       </c>
       <c r="F133" s="1">
-        <v>0.8391430634791014</v>
+        <v>0.9600018500109168</v>
       </c>
       <c r="G133">
-        <v>2109.30829354</v>
+        <v>1722.58068332</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -3481,16 +3481,16 @@
         <v>8</v>
       </c>
       <c r="D134">
-        <v>1694</v>
+        <v>0</v>
       </c>
       <c r="E134">
-        <v>183855</v>
+        <v>208396.9999999813</v>
       </c>
       <c r="F134" s="1">
-        <v>0.8469466457471697</v>
+        <v>0.9600018500109168</v>
       </c>
       <c r="G134">
-        <v>2012.79001826</v>
+        <v>1722.58068332</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -3507,13 +3507,13 @@
         <v>0</v>
       </c>
       <c r="E135">
-        <v>183855</v>
+        <v>208396.9999999813</v>
       </c>
       <c r="F135" s="1">
-        <v>0.8469466457471697</v>
+        <v>0.9600018500109168</v>
       </c>
       <c r="G135">
-        <v>2012.79001826</v>
+        <v>1722.58068332</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -3527,16 +3527,16 @@
         <v>8</v>
       </c>
       <c r="D136">
-        <v>2012</v>
+        <v>0</v>
       </c>
       <c r="E136">
-        <v>185867</v>
+        <v>208396.9999999813</v>
       </c>
       <c r="F136" s="1">
-        <v>0.8562151271659144</v>
+        <v>0.9600018500109168</v>
       </c>
       <c r="G136">
-        <v>2012.79001826</v>
+        <v>1722.580683320061</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -3550,16 +3550,16 @@
         <v>8</v>
       </c>
       <c r="D137">
-        <v>0</v>
+        <v>1722</v>
       </c>
       <c r="E137">
-        <v>185867</v>
+        <v>210118.9999999813</v>
       </c>
       <c r="F137" s="1">
-        <v>0.8562151271659144</v>
+        <v>0.9679344171098623</v>
       </c>
       <c r="G137">
-        <v>2012.79001826</v>
+        <v>1722.58068332</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -3573,16 +3573,16 @@
         <v>8</v>
       </c>
       <c r="D138">
-        <v>2012</v>
+        <v>1722</v>
       </c>
       <c r="E138">
-        <v>187879</v>
+        <v>211840.9999999813</v>
       </c>
       <c r="F138" s="1">
-        <v>0.8654836085846591</v>
+        <v>0.9758669842088078</v>
       </c>
       <c r="G138">
-        <v>2012.79001826</v>
+        <v>1722.58068332</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -3596,16 +3596,16 @@
         <v>8</v>
       </c>
       <c r="D139">
-        <v>2012</v>
+        <v>0</v>
       </c>
       <c r="E139">
-        <v>189891</v>
+        <v>211840.9999999813</v>
       </c>
       <c r="F139" s="1">
-        <v>0.8747520900034038</v>
+        <v>0.9758669842088078</v>
       </c>
       <c r="G139">
-        <v>2012.79001826</v>
+        <v>1722.58068332</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -3619,16 +3619,16 @@
         <v>8</v>
       </c>
       <c r="D140">
-        <v>1916</v>
+        <v>1722</v>
       </c>
       <c r="E140">
-        <v>191807</v>
+        <v>213562.9999999813</v>
       </c>
       <c r="F140" s="1">
-        <v>0.8835783377162839</v>
+        <v>0.9837995513077533</v>
       </c>
       <c r="G140">
-        <v>1916.27174298</v>
+        <v>1722.58068332</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -3642,16 +3642,16 @@
         <v>8</v>
       </c>
       <c r="D141">
-        <v>1916</v>
+        <v>1722.000000018698</v>
       </c>
       <c r="E141">
-        <v>193723</v>
+        <v>215285</v>
       </c>
       <c r="F141" s="1">
-        <v>0.892404585429164</v>
+        <v>0.9917321184067849</v>
       </c>
       <c r="G141">
-        <v>1916.27174298</v>
+        <v>1722.58068332</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -3665,16 +3665,16 @@
         <v>8</v>
       </c>
       <c r="D142">
-        <v>1916</v>
+        <v>0</v>
       </c>
       <c r="E142">
-        <v>195639</v>
+        <v>215285</v>
       </c>
       <c r="F142" s="1">
-        <v>0.9012308331420442</v>
+        <v>0.9917321184067849</v>
       </c>
       <c r="G142">
-        <v>1916.27174298</v>
+        <v>1722.58068332</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -3688,16 +3688,16 @@
         <v>8</v>
       </c>
       <c r="D143">
-        <v>1916</v>
+        <v>0</v>
       </c>
       <c r="E143">
-        <v>197555</v>
+        <v>215285</v>
       </c>
       <c r="F143" s="1">
-        <v>0.9100570808549243</v>
+        <v>0.9917321184067849</v>
       </c>
       <c r="G143">
-        <v>1916.27174298</v>
+        <v>1722.58068332</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -3711,16 +3711,16 @@
         <v>8</v>
       </c>
       <c r="D144">
-        <v>1916</v>
+        <v>0</v>
       </c>
       <c r="E144">
-        <v>199471</v>
+        <v>215285</v>
       </c>
       <c r="F144" s="1">
-        <v>0.9188833285678044</v>
+        <v>0.9917321184067849</v>
       </c>
       <c r="G144">
-        <v>1916.27174298</v>
+        <v>1722.58068332</v>
       </c>
     </row>
     <row r="145" spans="1:7">
@@ -3734,16 +3734,16 @@
         <v>8</v>
       </c>
       <c r="D145">
-        <v>1819</v>
+        <v>0</v>
       </c>
       <c r="E145">
-        <v>201290</v>
+        <v>215285</v>
       </c>
       <c r="F145" s="1">
-        <v>0.9272627359737173</v>
+        <v>0.9917321184067849</v>
       </c>
       <c r="G145">
-        <v>1819.7534677</v>
+        <v>1722.58068332</v>
       </c>
     </row>
     <row r="146" spans="1:7">
@@ -3757,16 +3757,16 @@
         <v>8</v>
       </c>
       <c r="D146">
-        <v>1819</v>
+        <v>0</v>
       </c>
       <c r="E146">
-        <v>203109</v>
+        <v>215285</v>
       </c>
       <c r="F146" s="1">
-        <v>0.9356421433796301</v>
+        <v>0.9917321184067849</v>
       </c>
       <c r="G146">
-        <v>1819.7534677</v>
+        <v>1722.58068332</v>
       </c>
     </row>
     <row r="147" spans="1:7">
@@ -3780,16 +3780,16 @@
         <v>8</v>
       </c>
       <c r="D147">
-        <v>1819</v>
+        <v>0</v>
       </c>
       <c r="E147">
-        <v>204928</v>
+        <v>215285</v>
       </c>
       <c r="F147" s="1">
-        <v>0.944021550785543</v>
+        <v>0.9917321184067849</v>
       </c>
       <c r="G147">
-        <v>1819.7534677</v>
+        <v>1722.58068332</v>
       </c>
     </row>
     <row r="148" spans="1:7">
@@ -3803,16 +3803,16 @@
         <v>8</v>
       </c>
       <c r="D148">
-        <v>1819</v>
+        <v>0</v>
       </c>
       <c r="E148">
-        <v>206747</v>
+        <v>215285</v>
       </c>
       <c r="F148" s="1">
-        <v>0.9524009581914558</v>
+        <v>0.9917321184067849</v>
       </c>
       <c r="G148">
-        <v>1819.7534677</v>
+        <v>1722.58068332</v>
       </c>
     </row>
     <row r="149" spans="1:7">
@@ -3826,13 +3826,13 @@
         <v>8</v>
       </c>
       <c r="D149">
-        <v>1722</v>
+        <v>0</v>
       </c>
       <c r="E149">
-        <v>208469</v>
+        <v>215285</v>
       </c>
       <c r="F149" s="1">
-        <v>0.9603335252904013</v>
+        <v>0.9917321184067849</v>
       </c>
       <c r="G149">
         <v>1722.58068332</v>
@@ -3849,13 +3849,13 @@
         <v>8</v>
       </c>
       <c r="D150">
-        <v>1722</v>
+        <v>0</v>
       </c>
       <c r="E150">
-        <v>210191</v>
+        <v>215285</v>
       </c>
       <c r="F150" s="1">
-        <v>0.9682660923893468</v>
+        <v>0.9917321184067849</v>
       </c>
       <c r="G150">
         <v>1722.58068332</v>
@@ -3875,10 +3875,10 @@
         <v>1722</v>
       </c>
       <c r="E151">
-        <v>211913</v>
+        <v>217007</v>
       </c>
       <c r="F151" s="1">
-        <v>0.9761986594882922</v>
+        <v>0.9996646855057304</v>
       </c>
       <c r="G151">
         <v>1722.58068332</v>
@@ -3895,16 +3895,16 @@
         <v>8</v>
       </c>
       <c r="D152">
-        <v>1722</v>
+        <v>0</v>
       </c>
       <c r="E152">
-        <v>213635</v>
+        <v>217007</v>
       </c>
       <c r="F152" s="1">
-        <v>0.9841312265872377</v>
+        <v>0.9996646855057304</v>
       </c>
       <c r="G152">
-        <v>1722.580683320142</v>
+        <v>1722.58068332</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -3918,13 +3918,13 @@
         <v>8</v>
       </c>
       <c r="D153">
-        <v>1722</v>
+        <v>72</v>
       </c>
       <c r="E153">
-        <v>215357</v>
+        <v>217079</v>
       </c>
       <c r="F153" s="1">
-        <v>0.9920637936861832</v>
+        <v>0.9999963607851288</v>
       </c>
       <c r="G153">
         <v>1722.58068332</v>
@@ -3941,7 +3941,7 @@
         <v>8</v>
       </c>
       <c r="D154">
-        <v>1722</v>
+        <v>0</v>
       </c>
       <c r="E154">
         <v>217079</v>
@@ -4608,7 +4608,7 @@
         <v>9</v>
       </c>
       <c r="D183">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E183">
         <v>217079</v>
@@ -6172,13 +6172,13 @@
         <v>12</v>
       </c>
       <c r="D251">
-        <v>-3634.999999908693</v>
+        <v>-3635</v>
       </c>
       <c r="E251">
-        <v>195269.0000000913</v>
+        <v>195269</v>
       </c>
       <c r="F251" s="1">
-        <v>0.8995263907344451</v>
+        <v>0.8995263907340245</v>
       </c>
       <c r="G251">
         <v>-3635.322</v>
@@ -6198,10 +6198,10 @@
         <v>-3635</v>
       </c>
       <c r="E252">
-        <v>191634.0000000913</v>
+        <v>191634</v>
       </c>
       <c r="F252" s="1">
-        <v>0.8827813957259277</v>
+        <v>0.8827813957255072</v>
       </c>
       <c r="G252">
         <v>-3635.322</v>
@@ -6221,10 +6221,10 @@
         <v>-3635</v>
       </c>
       <c r="E253">
-        <v>187999.0000000913</v>
+        <v>187999</v>
       </c>
       <c r="F253" s="1">
-        <v>0.8660364007174104</v>
+        <v>0.8660364007169898</v>
       </c>
       <c r="G253">
         <v>-3635.322</v>
@@ -6244,10 +6244,10 @@
         <v>-3635</v>
       </c>
       <c r="E254">
-        <v>184364.0000000913</v>
+        <v>184364</v>
       </c>
       <c r="F254" s="1">
-        <v>0.8492914057088929</v>
+        <v>0.8492914057084724</v>
       </c>
       <c r="G254">
         <v>-3635.322</v>
@@ -6267,10 +6267,10 @@
         <v>-3635</v>
       </c>
       <c r="E255">
-        <v>180729.0000000913</v>
+        <v>180729</v>
       </c>
       <c r="F255" s="1">
-        <v>0.8325464107003756</v>
+        <v>0.8325464106999551</v>
       </c>
       <c r="G255">
         <v>-3635.322</v>
@@ -6290,10 +6290,10 @@
         <v>-3635</v>
       </c>
       <c r="E256">
-        <v>177094.0000000913</v>
+        <v>177094</v>
       </c>
       <c r="F256" s="1">
-        <v>0.8158014156918583</v>
+        <v>0.8158014156914377</v>
       </c>
       <c r="G256">
         <v>-3635.322</v>
@@ -6313,10 +6313,10 @@
         <v>-3635</v>
       </c>
       <c r="E257">
-        <v>173459.0000000913</v>
+        <v>173459</v>
       </c>
       <c r="F257" s="1">
-        <v>0.7990564206833408</v>
+        <v>0.7990564206829203</v>
       </c>
       <c r="G257">
         <v>-3635.322</v>
@@ -6336,10 +6336,10 @@
         <v>-3635</v>
       </c>
       <c r="E258">
-        <v>169824.0000000913</v>
+        <v>169824</v>
       </c>
       <c r="F258" s="1">
-        <v>0.7823114256748235</v>
+        <v>0.7823114256744029</v>
       </c>
       <c r="G258">
         <v>-3635.322</v>
@@ -6359,10 +6359,10 @@
         <v>-3635</v>
       </c>
       <c r="E259">
-        <v>166189.0000000913</v>
+        <v>166189</v>
       </c>
       <c r="F259" s="1">
-        <v>0.7655664306663061</v>
+        <v>0.7655664306658856</v>
       </c>
       <c r="G259">
         <v>-3635.322</v>
@@ -6382,10 +6382,10 @@
         <v>-3635</v>
       </c>
       <c r="E260">
-        <v>162554.0000000913</v>
+        <v>162554</v>
       </c>
       <c r="F260" s="1">
-        <v>0.7488214356577887</v>
+        <v>0.7488214356573683</v>
       </c>
       <c r="G260">
         <v>-3635.322</v>
@@ -6402,13 +6402,13 @@
         <v>12</v>
       </c>
       <c r="D261">
-        <v>-3635</v>
+        <v>-3635.000000043614</v>
       </c>
       <c r="E261">
-        <v>158919.0000000913</v>
+        <v>158918.9999999564</v>
       </c>
       <c r="F261" s="1">
-        <v>0.7320764406492714</v>
+        <v>0.73207644064865</v>
       </c>
       <c r="G261">
         <v>-3635.322</v>
@@ -6428,10 +6428,10 @@
         <v>-3635</v>
       </c>
       <c r="E262">
-        <v>155284.0000000913</v>
+        <v>155283.9999999564</v>
       </c>
       <c r="F262" s="1">
-        <v>0.715331445640754</v>
+        <v>0.7153314456401326</v>
       </c>
       <c r="G262">
         <v>-3635.322</v>
@@ -6451,10 +6451,10 @@
         <v>-3635</v>
       </c>
       <c r="E263">
-        <v>151649.0000000913</v>
+        <v>151648.9999999564</v>
       </c>
       <c r="F263" s="1">
-        <v>0.6985864506322366</v>
+        <v>0.6985864506316152</v>
       </c>
       <c r="G263">
         <v>-3635.322</v>
@@ -6474,10 +6474,10 @@
         <v>-3635</v>
       </c>
       <c r="E264">
-        <v>148014.0000000913</v>
+        <v>148013.9999999564</v>
       </c>
       <c r="F264" s="1">
-        <v>0.6818414556237192</v>
+        <v>0.6818414556230978</v>
       </c>
       <c r="G264">
         <v>-3635.322</v>
@@ -6497,10 +6497,10 @@
         <v>-3635</v>
       </c>
       <c r="E265">
-        <v>144379.0000000913</v>
+        <v>144378.9999999564</v>
       </c>
       <c r="F265" s="1">
-        <v>0.6650964606152019</v>
+        <v>0.6650964606145805</v>
       </c>
       <c r="G265">
         <v>-3635.322</v>
@@ -6520,10 +6520,10 @@
         <v>-3635</v>
       </c>
       <c r="E266">
-        <v>140744.0000000913</v>
+        <v>140743.9999999564</v>
       </c>
       <c r="F266" s="1">
-        <v>0.6483514656066846</v>
+        <v>0.648351465606063</v>
       </c>
       <c r="G266">
         <v>-3635.322</v>
@@ -6543,10 +6543,10 @@
         <v>-3635</v>
       </c>
       <c r="E267">
-        <v>137109.0000000913</v>
+        <v>137108.9999999564</v>
       </c>
       <c r="F267" s="1">
-        <v>0.6316064705981671</v>
+        <v>0.6316064705975457</v>
       </c>
       <c r="G267">
         <v>-3635.322</v>
@@ -6566,10 +6566,10 @@
         <v>-3635</v>
       </c>
       <c r="E268">
-        <v>133474.0000000913</v>
+        <v>133473.9999999564</v>
       </c>
       <c r="F268" s="1">
-        <v>0.6148614755896498</v>
+        <v>0.6148614755890284</v>
       </c>
       <c r="G268">
         <v>-3635.322</v>
@@ -6589,10 +6589,10 @@
         <v>-3635</v>
       </c>
       <c r="E269">
-        <v>129839.0000000913</v>
+        <v>129838.9999999564</v>
       </c>
       <c r="F269" s="1">
-        <v>0.5981164805811324</v>
+        <v>0.5981164805805109</v>
       </c>
       <c r="G269">
         <v>-3635.322</v>
@@ -6612,10 +6612,10 @@
         <v>-3635</v>
       </c>
       <c r="E270">
-        <v>126204.0000000913</v>
+        <v>126203.9999999564</v>
       </c>
       <c r="F270" s="1">
-        <v>0.5813714855726151</v>
+        <v>0.5813714855719935</v>
       </c>
       <c r="G270">
         <v>-3635.322</v>
@@ -6635,10 +6635,10 @@
         <v>-3635</v>
       </c>
       <c r="E271">
-        <v>122569.0000000913</v>
+        <v>122568.9999999564</v>
       </c>
       <c r="F271" s="1">
-        <v>0.5646264905640976</v>
+        <v>0.5646264905634761</v>
       </c>
       <c r="G271">
         <v>-3635.322</v>
@@ -6658,10 +6658,10 @@
         <v>-3635</v>
       </c>
       <c r="E272">
-        <v>118934.0000000913</v>
+        <v>118933.9999999564</v>
       </c>
       <c r="F272" s="1">
-        <v>0.5478814955555803</v>
+        <v>0.5478814955549588</v>
       </c>
       <c r="G272">
         <v>-3635.322</v>
@@ -6678,13 +6678,13 @@
         <v>12</v>
       </c>
       <c r="D273">
-        <v>-3635</v>
+        <v>-3150</v>
       </c>
       <c r="E273">
-        <v>115299.0000000913</v>
+        <v>115783.9999999564</v>
       </c>
       <c r="F273" s="1">
-        <v>0.531136500547063</v>
+        <v>0.533370702081278</v>
       </c>
       <c r="G273">
         <v>-3635.322</v>
@@ -6704,10 +6704,10 @@
         <v>-3635</v>
       </c>
       <c r="E274">
-        <v>111664.0000000913</v>
+        <v>112148.9999999564</v>
       </c>
       <c r="F274" s="1">
-        <v>0.5143915055385456</v>
+        <v>0.5166257070727606</v>
       </c>
       <c r="G274">
         <v>-3635.322</v>
@@ -6724,13 +6724,13 @@
         <v>12</v>
       </c>
       <c r="D275">
-        <v>-3150.000000091307</v>
+        <v>-3635</v>
       </c>
       <c r="E275">
-        <v>108514</v>
+        <v>108513.9999999564</v>
       </c>
       <c r="F275" s="1">
-        <v>0.4998807120644441</v>
+        <v>0.4998807120642432</v>
       </c>
       <c r="G275">
         <v>-3635.322</v>
@@ -6750,10 +6750,10 @@
         <v>-3635</v>
       </c>
       <c r="E276">
-        <v>104879</v>
+        <v>104878.9999999564</v>
       </c>
       <c r="F276" s="1">
-        <v>0.4831357170559267</v>
+        <v>0.4831357170557258</v>
       </c>
       <c r="G276">
         <v>-3635.322</v>
@@ -6773,10 +6773,10 @@
         <v>-3635</v>
       </c>
       <c r="E277">
-        <v>101244</v>
+        <v>101243.9999999564</v>
       </c>
       <c r="F277" s="1">
-        <v>0.4663907220474094</v>
+        <v>0.4663907220472085</v>
       </c>
       <c r="G277">
         <v>-3635.322</v>
@@ -6796,10 +6796,10 @@
         <v>-3635</v>
       </c>
       <c r="E278">
-        <v>97609</v>
+        <v>97608.99999995639</v>
       </c>
       <c r="F278" s="1">
-        <v>0.449645727038892</v>
+        <v>0.4496457270386911</v>
       </c>
       <c r="G278">
         <v>-3635.322</v>
@@ -6819,10 +6819,10 @@
         <v>-3635</v>
       </c>
       <c r="E279">
-        <v>93974</v>
+        <v>93973.99999995639</v>
       </c>
       <c r="F279" s="1">
-        <v>0.4329007320303746</v>
+        <v>0.4329007320301737</v>
       </c>
       <c r="G279">
         <v>-3635.322</v>
@@ -6842,10 +6842,10 @@
         <v>-3635</v>
       </c>
       <c r="E280">
-        <v>90339</v>
+        <v>90338.99999995639</v>
       </c>
       <c r="F280" s="1">
-        <v>0.4161557370218573</v>
+        <v>0.4161557370216564</v>
       </c>
       <c r="G280">
         <v>-3635.322</v>
@@ -6865,10 +6865,10 @@
         <v>-3635</v>
       </c>
       <c r="E281">
-        <v>86704</v>
+        <v>86703.99999995639</v>
       </c>
       <c r="F281" s="1">
-        <v>0.3994107420133399</v>
+        <v>0.399410742013139</v>
       </c>
       <c r="G281">
         <v>-3635.322</v>
@@ -6888,10 +6888,10 @@
         <v>-3635</v>
       </c>
       <c r="E282">
-        <v>83069</v>
+        <v>83068.99999995639</v>
       </c>
       <c r="F282" s="1">
-        <v>0.3826657470048225</v>
+        <v>0.3826657470046216</v>
       </c>
       <c r="G282">
         <v>-3635.322</v>
@@ -6911,10 +6911,10 @@
         <v>-3635</v>
       </c>
       <c r="E283">
-        <v>79434</v>
+        <v>79433.99999995639</v>
       </c>
       <c r="F283" s="1">
-        <v>0.3659207519963051</v>
+        <v>0.3659207519961042</v>
       </c>
       <c r="G283">
         <v>-3635.322</v>
@@ -6934,10 +6934,10 @@
         <v>-3635</v>
       </c>
       <c r="E284">
-        <v>75799</v>
+        <v>75798.99999995639</v>
       </c>
       <c r="F284" s="1">
-        <v>0.3491757569877877</v>
+        <v>0.3491757569875868</v>
       </c>
       <c r="G284">
         <v>-3635.322</v>
@@ -6957,10 +6957,10 @@
         <v>-3635</v>
       </c>
       <c r="E285">
-        <v>72164</v>
+        <v>72163.99999995639</v>
       </c>
       <c r="F285" s="1">
-        <v>0.3324307619792704</v>
+        <v>0.3324307619790695</v>
       </c>
       <c r="G285">
         <v>-3635.322</v>
@@ -6980,10 +6980,10 @@
         <v>-3635</v>
       </c>
       <c r="E286">
-        <v>68529</v>
+        <v>68528.99999995639</v>
       </c>
       <c r="F286" s="1">
-        <v>0.315685766970753</v>
+        <v>0.3156857669705521</v>
       </c>
       <c r="G286">
         <v>-3635.322</v>
@@ -7003,10 +7003,10 @@
         <v>-3635</v>
       </c>
       <c r="E287">
-        <v>64894</v>
+        <v>64893.99999995639</v>
       </c>
       <c r="F287" s="1">
-        <v>0.2989407719622356</v>
+        <v>0.2989407719620347</v>
       </c>
       <c r="G287">
         <v>-3635.322</v>
@@ -7026,10 +7026,10 @@
         <v>-3635</v>
       </c>
       <c r="E288">
-        <v>61259</v>
+        <v>61258.99999995639</v>
       </c>
       <c r="F288" s="1">
-        <v>0.2821957769537182</v>
+        <v>0.2821957769535173</v>
       </c>
       <c r="G288">
         <v>-3635.322</v>
@@ -7049,10 +7049,10 @@
         <v>-3635</v>
       </c>
       <c r="E289">
-        <v>57624</v>
+        <v>57623.99999995639</v>
       </c>
       <c r="F289" s="1">
-        <v>0.2654507819452009</v>
+        <v>0.265450781945</v>
       </c>
       <c r="G289">
         <v>-3635.322</v>
@@ -7072,10 +7072,10 @@
         <v>-3635</v>
       </c>
       <c r="E290">
-        <v>53989</v>
+        <v>53988.99999995639</v>
       </c>
       <c r="F290" s="1">
-        <v>0.2487057869366835</v>
+        <v>0.2487057869364826</v>
       </c>
       <c r="G290">
         <v>-3635.322</v>
@@ -7095,10 +7095,10 @@
         <v>-3635</v>
       </c>
       <c r="E291">
-        <v>50354</v>
+        <v>50353.99999995639</v>
       </c>
       <c r="F291" s="1">
-        <v>0.2319607919281661</v>
+        <v>0.2319607919279652</v>
       </c>
       <c r="G291">
         <v>-3635.322</v>
@@ -7118,10 +7118,10 @@
         <v>-3469</v>
       </c>
       <c r="E292">
-        <v>46885</v>
+        <v>46884.99999995639</v>
       </c>
       <c r="F292" s="1">
-        <v>0.2159804927027062</v>
+        <v>0.2159804927025053</v>
       </c>
       <c r="G292">
         <v>-3469.58767002</v>
@@ -7138,16 +7138,16 @@
         <v>1</v>
       </c>
       <c r="D293">
-        <v>-3469</v>
+        <v>-3468.999999991574</v>
       </c>
       <c r="E293">
-        <v>43416</v>
+        <v>43415.99999996481</v>
       </c>
       <c r="F293" s="1">
-        <v>0.2000001934772463</v>
+        <v>0.2000001934770842</v>
       </c>
       <c r="G293">
-        <v>-3469.58767002</v>
+        <v>-3469.587670011568</v>
       </c>
     </row>
     <row r="294" spans="1:7">
@@ -7164,10 +7164,10 @@
         <v>-3055</v>
       </c>
       <c r="E294">
-        <v>40361</v>
+        <v>40360.99999996481</v>
       </c>
       <c r="F294" s="1">
-        <v>0.1859270271083273</v>
+        <v>0.1859270271081652</v>
       </c>
       <c r="G294">
         <v>-3055.27002168</v>
@@ -7187,10 +7187,10 @@
         <v>-3055</v>
       </c>
       <c r="E295">
-        <v>37306</v>
+        <v>37305.99999996481</v>
       </c>
       <c r="F295" s="1">
-        <v>0.1718538607394083</v>
+        <v>0.1718538607392462</v>
       </c>
       <c r="G295">
         <v>-3055.27002168</v>
@@ -7210,10 +7210,10 @@
         <v>-2806</v>
       </c>
       <c r="E296">
-        <v>34500</v>
+        <v>34499.99999996481</v>
       </c>
       <c r="F296" s="1">
-        <v>0.1589277380450755</v>
+        <v>0.1589277380449134</v>
       </c>
       <c r="G296">
         <v>-2806.686703320001</v>
@@ -7233,10 +7233,10 @@
         <v>-2806</v>
       </c>
       <c r="E297">
-        <v>31694</v>
+        <v>31693.99999996481</v>
       </c>
       <c r="F297" s="1">
-        <v>0.1460016153507427</v>
+        <v>0.1460016153505806</v>
       </c>
       <c r="G297">
         <v>-2806.686703320001</v>
@@ -7256,10 +7256,10 @@
         <v>-2806</v>
       </c>
       <c r="E298">
-        <v>28888</v>
+        <v>28887.99999996481</v>
       </c>
       <c r="F298" s="1">
-        <v>0.1330754926564099</v>
+        <v>0.1330754926562478</v>
       </c>
       <c r="G298">
         <v>-2806.686703320001</v>
@@ -7279,10 +7279,10 @@
         <v>-2806</v>
       </c>
       <c r="E299">
-        <v>26082</v>
+        <v>26081.99999996481</v>
       </c>
       <c r="F299" s="1">
-        <v>0.1201493699620771</v>
+        <v>0.120149369961915</v>
       </c>
       <c r="G299">
         <v>-2806.686703320001</v>
@@ -7302,10 +7302,10 @@
         <v>-2475</v>
       </c>
       <c r="E300">
-        <v>23607</v>
+        <v>23606.99999996481</v>
       </c>
       <c r="F300" s="1">
-        <v>0.1087480322327564</v>
+        <v>0.1087480322325943</v>
       </c>
       <c r="G300">
         <v>-2475.25439658</v>
@@ -7325,10 +7325,10 @@
         <v>-2475</v>
       </c>
       <c r="E301">
-        <v>21132</v>
+        <v>21131.99999996481</v>
       </c>
       <c r="F301" s="1">
-        <v>0.0973466945034358</v>
+        <v>0.0973466945032737</v>
       </c>
       <c r="G301">
         <v>-2475.25439658</v>
@@ -7348,10 +7348,10 @@
         <v>-2475</v>
       </c>
       <c r="E302">
-        <v>18657</v>
+        <v>18656.99999996481</v>
       </c>
       <c r="F302" s="1">
-        <v>0.08594535677411518</v>
+        <v>0.08594535677395307</v>
       </c>
       <c r="G302">
         <v>-2475.25439658</v>
@@ -7371,10 +7371,10 @@
         <v>-2143</v>
       </c>
       <c r="E303">
-        <v>16514</v>
+        <v>16513.99999996481</v>
       </c>
       <c r="F303" s="1">
-        <v>0.07607341061090947</v>
+        <v>0.07607341061074736</v>
       </c>
       <c r="G303">
         <v>-2143.78573662</v>
@@ -7394,10 +7394,10 @@
         <v>-2143</v>
       </c>
       <c r="E304">
-        <v>14371</v>
+        <v>14370.99999996481</v>
       </c>
       <c r="F304" s="1">
-        <v>0.06620146444770376</v>
+        <v>0.06620146444754167</v>
       </c>
       <c r="G304">
         <v>-2143.78573662</v>
@@ -7417,10 +7417,10 @@
         <v>-2143</v>
       </c>
       <c r="E305">
-        <v>12228</v>
+        <v>12227.99999996481</v>
       </c>
       <c r="F305" s="1">
-        <v>0.05632951828449806</v>
+        <v>0.05632951828433597</v>
       </c>
       <c r="G305">
         <v>-2143.78573662</v>
@@ -7440,10 +7440,10 @@
         <v>-2143</v>
       </c>
       <c r="E306">
-        <v>10085</v>
+        <v>10084.99999996481</v>
       </c>
       <c r="F306" s="1">
-        <v>0.04645757212129236</v>
+        <v>0.04645757212113026</v>
       </c>
       <c r="G306">
         <v>-2143.78573662</v>
@@ -7463,10 +7463,10 @@
         <v>-1812</v>
       </c>
       <c r="E307">
-        <v>8273</v>
+        <v>8272.999999964812</v>
       </c>
       <c r="F307" s="1">
-        <v>0.03811041092309883</v>
+        <v>0.03811041092293673</v>
       </c>
       <c r="G307">
         <v>-1812.35342988</v>
@@ -7483,16 +7483,16 @@
         <v>2</v>
       </c>
       <c r="D308">
-        <v>0</v>
+        <v>-1811.999999964812</v>
       </c>
       <c r="E308">
-        <v>8273</v>
+        <v>6461</v>
       </c>
       <c r="F308" s="1">
-        <v>0.03811041092309883</v>
+        <v>0.0297632497249053</v>
       </c>
       <c r="G308">
-        <v>-1812.35342988</v>
+        <v>-1812.353429844766</v>
       </c>
     </row>
     <row r="309" spans="1:7">
@@ -7509,10 +7509,10 @@
         <v>0</v>
       </c>
       <c r="E309">
-        <v>8273</v>
+        <v>6461</v>
       </c>
       <c r="F309" s="1">
-        <v>0.03811041092309883</v>
+        <v>0.0297632497249053</v>
       </c>
       <c r="G309">
         <v>-1812.35342988</v>
@@ -7532,10 +7532,10 @@
         <v>-1812</v>
       </c>
       <c r="E310">
-        <v>6461</v>
+        <v>4649</v>
       </c>
       <c r="F310" s="1">
-        <v>0.0297632497249053</v>
+        <v>0.02141608852671177</v>
       </c>
       <c r="G310">
         <v>-1812.35342988</v>
@@ -7555,10 +7555,10 @@
         <v>-1812</v>
       </c>
       <c r="E311">
-        <v>4649</v>
+        <v>2837</v>
       </c>
       <c r="F311" s="1">
-        <v>0.02141608852671177</v>
+        <v>0.01306892732851824</v>
       </c>
       <c r="G311">
         <v>-1812.35342988</v>
@@ -7575,13 +7575,13 @@
         <v>2</v>
       </c>
       <c r="D312">
-        <v>-1812</v>
+        <v>-1025</v>
       </c>
       <c r="E312">
-        <v>2837</v>
+        <v>1812</v>
       </c>
       <c r="F312" s="1">
-        <v>0.01306892732851824</v>
+        <v>0.00834716119819353</v>
       </c>
       <c r="G312">
         <v>-1812.35342988</v>
@@ -7601,10 +7601,10 @@
         <v>0</v>
       </c>
       <c r="E313">
-        <v>2837</v>
+        <v>1812</v>
       </c>
       <c r="F313" s="1">
-        <v>0.01306892732851824</v>
+        <v>0.00834716119819353</v>
       </c>
       <c r="G313">
         <v>-1812.35342988</v>
@@ -7624,10 +7624,10 @@
         <v>0</v>
       </c>
       <c r="E314">
-        <v>2837</v>
+        <v>1812</v>
       </c>
       <c r="F314" s="1">
-        <v>0.01306892732851824</v>
+        <v>0.00834716119819353</v>
       </c>
       <c r="G314">
         <v>-1812.35342988</v>
@@ -7644,13 +7644,13 @@
         <v>2</v>
       </c>
       <c r="D315">
-        <v>-1812</v>
+        <v>0</v>
       </c>
       <c r="E315">
-        <v>1025</v>
+        <v>1812</v>
       </c>
       <c r="F315" s="1">
-        <v>0.004721766130324706</v>
+        <v>0.00834716119819353</v>
       </c>
       <c r="G315">
         <v>-1812.35342988</v>
@@ -7670,10 +7670,10 @@
         <v>0</v>
       </c>
       <c r="E316">
-        <v>1025</v>
+        <v>1812</v>
       </c>
       <c r="F316" s="1">
-        <v>0.004721766130324706</v>
+        <v>0.00834716119819353</v>
       </c>
       <c r="G316">
         <v>-1812.35342988</v>
@@ -7690,13 +7690,13 @@
         <v>2</v>
       </c>
       <c r="D317">
-        <v>0</v>
+        <v>-1812</v>
       </c>
       <c r="E317">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="F317" s="1">
-        <v>0.004721766130324706</v>
+        <v>0</v>
       </c>
       <c r="G317">
         <v>-1812.35342988</v>
@@ -7716,10 +7716,10 @@
         <v>0</v>
       </c>
       <c r="E318">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="F318" s="1">
-        <v>0.004721766130324706</v>
+        <v>0</v>
       </c>
       <c r="G318">
         <v>-1812.35342988</v>
@@ -7739,10 +7739,10 @@
         <v>0</v>
       </c>
       <c r="E319">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="F319" s="1">
-        <v>0.004721766130324706</v>
+        <v>0</v>
       </c>
       <c r="G319">
         <v>-1812.35342988</v>
@@ -7762,10 +7762,10 @@
         <v>0</v>
       </c>
       <c r="E320">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="F320" s="1">
-        <v>0.004721766130324706</v>
+        <v>0</v>
       </c>
       <c r="G320">
         <v>-1812.35342988</v>
@@ -7785,10 +7785,10 @@
         <v>0</v>
       </c>
       <c r="E321">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="F321" s="1">
-        <v>0.004721766130324706</v>
+        <v>0</v>
       </c>
       <c r="G321">
         <v>-1812.35342988</v>
@@ -7808,10 +7808,10 @@
         <v>0</v>
       </c>
       <c r="E322">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="F322" s="1">
-        <v>0.004721766130324706</v>
+        <v>0</v>
       </c>
       <c r="G322">
         <v>-1812.35342988</v>
@@ -7831,10 +7831,10 @@
         <v>0</v>
       </c>
       <c r="E323">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="F323" s="1">
-        <v>0.004721766130324706</v>
+        <v>0</v>
       </c>
       <c r="G323">
         <v>-1812.35342988</v>
@@ -7854,10 +7854,10 @@
         <v>0</v>
       </c>
       <c r="E324">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="F324" s="1">
-        <v>0.004721766130324706</v>
+        <v>0</v>
       </c>
       <c r="G324">
         <v>-1812.35342988</v>
@@ -7877,10 +7877,10 @@
         <v>0</v>
       </c>
       <c r="E325">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="F325" s="1">
-        <v>0.004721766130324706</v>
+        <v>0</v>
       </c>
       <c r="G325">
         <v>-1812.35342988</v>
@@ -7900,10 +7900,10 @@
         <v>0</v>
       </c>
       <c r="E326">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="F326" s="1">
-        <v>0.004721766130324706</v>
+        <v>0</v>
       </c>
       <c r="G326">
         <v>-1812.35342988</v>
@@ -7923,10 +7923,10 @@
         <v>0</v>
       </c>
       <c r="E327">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="F327" s="1">
-        <v>0.004721766130324706</v>
+        <v>0</v>
       </c>
       <c r="G327">
         <v>-1812.35342988</v>
@@ -7946,10 +7946,10 @@
         <v>0</v>
       </c>
       <c r="E328">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="F328" s="1">
-        <v>0.004721766130324706</v>
+        <v>0</v>
       </c>
       <c r="G328">
         <v>-1812.35342988</v>
@@ -7969,10 +7969,10 @@
         <v>0</v>
       </c>
       <c r="E329">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="F329" s="1">
-        <v>0.004721766130324706</v>
+        <v>0</v>
       </c>
       <c r="G329">
         <v>-1812.35342988</v>
@@ -7992,10 +7992,10 @@
         <v>0</v>
       </c>
       <c r="E330">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="F330" s="1">
-        <v>0.004721766130324706</v>
+        <v>0</v>
       </c>
       <c r="G330">
         <v>-1812.35342988</v>
@@ -8015,10 +8015,10 @@
         <v>0</v>
       </c>
       <c r="E331">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="F331" s="1">
-        <v>0.004721766130324706</v>
+        <v>0</v>
       </c>
       <c r="G331">
         <v>-1812.35342988</v>
@@ -8038,10 +8038,10 @@
         <v>0</v>
       </c>
       <c r="E332">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="F332" s="1">
-        <v>0.004721766130324706</v>
+        <v>0</v>
       </c>
       <c r="G332">
         <v>-1812.35342988</v>
@@ -8058,7 +8058,7 @@
         <v>2</v>
       </c>
       <c r="D333">
-        <v>-1025</v>
+        <v>0</v>
       </c>
       <c r="E333">
         <v>0</v>
@@ -8590,10 +8590,10 @@
         <v>0</v>
       </c>
       <c r="E356">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F356" s="1">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="G356">
         <v>-1812.35342988</v>
@@ -8613,10 +8613,10 @@
         <v>0</v>
       </c>
       <c r="E357">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F357" s="1">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="G357">
         <v>-1812.35342988</v>
@@ -8636,10 +8636,10 @@
         <v>0</v>
       </c>
       <c r="E358">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F358" s="1">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="G358">
         <v>-1812.35342988</v>
@@ -8659,10 +8659,10 @@
         <v>0</v>
       </c>
       <c r="E359">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F359" s="1">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="G359">
         <v>-1812.35342988</v>
@@ -8682,10 +8682,10 @@
         <v>0</v>
       </c>
       <c r="E360">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F360" s="1">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="G360">
         <v>-1812.35342988</v>
@@ -8705,10 +8705,10 @@
         <v>0</v>
       </c>
       <c r="E361">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F361" s="1">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="G361">
         <v>-1812.35342988</v>
@@ -8870,13 +8870,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>8673</v>
+        <v>8673.000000013044</v>
       </c>
       <c r="D2">
-        <v>8673</v>
+        <v>8673.000000013044</v>
       </c>
       <c r="E2" s="1">
-        <v>0.03995305136420115</v>
+        <v>0.03995305136426124</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -8887,13 +8887,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>34120</v>
+        <v>67610.99999996826</v>
       </c>
       <c r="D3">
-        <v>42793</v>
+        <v>76283.9999999813</v>
       </c>
       <c r="E3" s="1">
-        <v>0.1971302809902294</v>
+        <v>0.3514099585225382</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -8907,10 +8907,10 @@
         <v>65430</v>
       </c>
       <c r="D4">
-        <v>108223</v>
+        <v>141713.9999999813</v>
       </c>
       <c r="E4" s="1">
-        <v>0.4985401911435422</v>
+        <v>0.652819868675851</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -8921,13 +8921,13 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>67611</v>
+        <v>64042</v>
       </c>
       <c r="D5">
-        <v>175834</v>
+        <v>205755.9999999813</v>
       </c>
       <c r="E5" s="1">
-        <v>0.8099970983019653</v>
+        <v>0.9478358164985387</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -8938,7 +8938,7 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>41245</v>
+        <v>11323.0000000187</v>
       </c>
       <c r="D6">
         <v>217079</v>
@@ -9006,13 +9006,13 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>-112200</v>
+        <v>-112200.0000000436</v>
       </c>
       <c r="D10">
-        <v>104879</v>
+        <v>104878.9999999564</v>
       </c>
       <c r="E10" s="1">
-        <v>0.4831357170559267</v>
+        <v>0.4831357170557258</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -9023,13 +9023,13 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>-96606</v>
+        <v>-96605.99999999157</v>
       </c>
       <c r="D11">
-        <v>8273</v>
+        <v>8272.999999964813</v>
       </c>
       <c r="E11" s="1">
-        <v>0.03811041092309883</v>
+        <v>0.03811041092293674</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -9040,13 +9040,13 @@
         <v>2</v>
       </c>
       <c r="C12">
-        <v>-8273</v>
+        <v>-8272.999999964812</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1.818989403545856E-12</v>
       </c>
       <c r="E12" s="1">
-        <v>0</v>
+        <v>8.379358592275479E-18</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -9060,10 +9060,10 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1.818989403545856E-12</v>
       </c>
       <c r="E13" s="1">
-        <v>0</v>
+        <v>8.379358592275479E-18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>